<commit_message>
updated project plan and COA template
</commit_message>
<xml_diff>
--- a/coa_template.xlsx
+++ b/coa_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <r>
       <rPr>
@@ -365,9 +365,6 @@
     <t xml:space="preserve">Whittier College</t>
   </si>
   <si>
-    <t xml:space="preserve">2017-Present</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -414,9 +411,6 @@
     <t xml:space="preserve">Last Active</t>
   </si>
   <si>
-    <t xml:space="preserve">R:</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b val="true"/>
@@ -606,15 +600,12 @@
     <t xml:space="preserve">Deaconu, Cosmin</t>
   </si>
   <si>
-    <t xml:space="preserve">Astronomy and Astrophysics</t>
+    <t xml:space="preserve">KICP</t>
   </si>
   <si>
     <t xml:space="preserve">Oberla, Eric</t>
   </si>
   <si>
-    <t xml:space="preserve">KICP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Smith, Dan</t>
   </si>
   <si>
@@ -640,9 +631,6 @@
   </si>
   <si>
     <t xml:space="preserve">Young, Robert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instrumentation and Design Lab</t>
   </si>
   <si>
     <t xml:space="preserve">Seckel, David </t>
@@ -691,7 +679,10 @@
     <t xml:space="preserve">Journal/Collection</t>
   </si>
   <si>
-    <t xml:space="preserve">B:</t>
+    <t xml:space="preserve">E:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astroparticle Physics</t>
   </si>
 </sst>
 </file>
@@ -703,7 +694,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -785,6 +776,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -836,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -900,6 +898,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -929,7 +934,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -990,6 +995,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1006,7 +1023,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1026,19 +1043,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1054,6 +1083,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1070,19 +1107,23 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1091,11 +1132,31 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1196,7 +1257,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableA" displayName="TableA" ref="A16:D17" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableA" displayName="TableA" ref="A16:D21" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="4">
     <tableColumn id="1" name="1"/>
     <tableColumn id="2" name="Your Name:"/>
@@ -1207,8 +1268,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableC" displayName="TableC" ref="A29:D30" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A29:D30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableC" displayName="TableC" ref="A37:D44" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A37:D44"/>
   <tableColumns count="4">
     <tableColumn id="1" name="3"/>
     <tableColumn id="2" name="Advisor/Advisee Name:"/>
@@ -1219,8 +1280,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableD" displayName="TableD" ref="A37:E42" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A37:E42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableD" displayName="TableD" ref="A51:E56" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A51:E56"/>
   <tableColumns count="5">
     <tableColumn id="1" name="4"/>
     <tableColumn id="2" name="Name:"/>
@@ -1232,8 +1293,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TableD23" displayName="TableD23" ref="A23:E24" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A23:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TableD23" displayName="TableD23" ref="A27:E32" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A27:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="2"/>
     <tableColumn id="2" name="Name"/>
@@ -1245,8 +1306,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TableD5" displayName="TableD5" ref="A58:E59" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A58:E59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TableD5" displayName="TableD5" ref="A77:E82" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A77:E82"/>
   <tableColumns count="5">
     <tableColumn id="1" name="5"/>
     <tableColumn id="2" name="Name:"/>
@@ -1262,10 +1323,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1437,524 +1498,632 @@
       <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" s="17" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="18"/>
+      <c r="B24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="18"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-    </row>
-    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19" t="s">
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="21" t="s">
+      <c r="B27" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="C27" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="D27" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="E27" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="23" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="27"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="31"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="30"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="31"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="34"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D36" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-    </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28"/>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="B37" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="21" t="s">
+      <c r="C37" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="D37" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="B38" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="C38" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="37"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="38"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="31"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="38"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="33"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="33"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="31"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="33"/>
+    </row>
+    <row r="45" s="21" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" s="21" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+    </row>
+    <row r="47" s="21" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="42"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="23"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="s">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E53" s="45"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="46"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E55" s="47"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="50"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="50"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="50"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" s="50"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="50"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" s="50"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="50"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="50"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" s="50"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="50"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="48"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="50"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="48"/>
+      <c r="B67" s="49"/>
+      <c r="C67" s="49"/>
+      <c r="D67" s="49"/>
+      <c r="E67" s="50"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="48"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="50"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="48"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="50"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="48"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="50"/>
+    </row>
+    <row r="71" s="21" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" s="21" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" s="21" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+    </row>
+    <row r="74" s="21" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+    </row>
+    <row r="75" s="21" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="51"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="23"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E77" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="13"/>
-    </row>
-    <row r="32" s="18" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-    </row>
-    <row r="33" s="18" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="34"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="20"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="36" t="n">
-        <v>44606</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E39" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E43" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E46" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="E50" s="36" t="n">
-        <v>44580</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="E51" s="36" t="n">
-        <v>43915</v>
-      </c>
-    </row>
-    <row r="52" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" s="18" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-    </row>
-    <row r="55" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16" t="s">
+      <c r="D78" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
-      <c r="E55" s="16"/>
-    </row>
-    <row r="56" s="18" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="41"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E57" s="20"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E58" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="36"/>
-    </row>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E78" s="16"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="31"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="46"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="31"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="46"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="31"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="46"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="52"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="54"/>
+      <c r="E82" s="55"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
     <mergeCell ref="A1:E1"/>
@@ -1971,34 +2140,34 @@
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="B24:E24"/>
     <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A54:E54"/>
-    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A74:E74"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A38:A51" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A52:A70" type="list">
       <formula1>"A:,C:"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A24" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A28:A32" type="list">
       <formula1>"R:"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A25" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A33" type="list">
       <formula1>"G:,T:,P:"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A59" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A78:A82" type="list">
       <formula1>"B:,E:"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A38:A44" type="list">
       <formula1>"G:,T:"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>